<commit_message>
Fix infrastructure costs, solution briefing logos, and SOW sign-off formatting
- Infrastructure Costs: Fix sheet names to match solution-template (mixed case)
- Infrastructure Costs: Increase Unit column width from 15 to 16 (5% rounded)
- Infrastructure Costs: Update metadata in disaster-recovery and onpremise-migration
- Solution Briefing: Fix logo paths to reference solution-local assets (../../assets/logos/)
- Statement of Work: Add sign-off table header vertical centering and subtle bottom padding
- Regenerate all 10 Office documents with fixes applied
</commit_message>
<xml_diff>
--- a/solutions/aws/cloud/disaster-recovery-web-application/presales/infrastructure-costs.xlsx
+++ b/solutions/aws/cloud/disaster-recovery-web-application/presales/infrastructure-costs.xlsx
@@ -7,16 +7,16 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cover" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SIZING GUIDELINES" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="INFRASTRUCTURE COSTS" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CREDITS" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SUMMARY" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sizing Guidelines" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Infrastructure Costs" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Credits" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="3-Year Summary" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SIZING GUIDELINES'!$A$2:$F$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'INFRASTRUCTURE COSTS'!$A$2:$K$26</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'CREDITS'!$A$2:$D$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'SUMMARY'!$A$2:$G$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sizing Guidelines'!$A$2:$F$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Infrastructure Costs'!$A$2:$K$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Credits'!$A$2:$D$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'3-Year Summary'!$A$2:$G$7</definedName>
   </definedNames>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
@@ -916,7 +916,7 @@
     <row r="1" ht="32" customHeight="1">
       <c r="A1" s="35" t="inlineStr">
         <is>
-          <t>SIZING GUIDELINES - Based on Solution Scope (Default: Small)</t>
+          <t>Sizing Guidelines</t>
         </is>
       </c>
     </row>
@@ -1204,7 +1204,7 @@
     <col width="30" customWidth="1" min="2" max="2"/>
     <col width="50" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="16" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
     <col width="15" customWidth="1" min="7" max="7"/>
     <col width="12" customWidth="1" min="8" max="8"/>
@@ -1216,7 +1216,7 @@
     <row r="1" ht="32" customHeight="1">
       <c r="A1" s="35" t="inlineStr">
         <is>
-          <t>INFRASTRUCTURE COSTS - Quantities Default to Small Scope</t>
+          <t>Infrastructure Costs</t>
         </is>
       </c>
     </row>
@@ -2466,7 +2466,7 @@
     <row r="1" ht="32" customHeight="1">
       <c r="A1" s="35" t="inlineStr">
         <is>
-          <t>CREDITS - Applied per Category (Year 1 Only)</t>
+          <t>Credits</t>
         </is>
       </c>
     </row>
@@ -2628,7 +2628,7 @@
     <row r="1" ht="32" customHeight="1">
       <c r="A1" s="35" t="inlineStr">
         <is>
-          <t>SUMMARY</t>
+          <t>3-Year Summary</t>
         </is>
       </c>
     </row>

</xml_diff>